<commit_message>
Stuck in the middle
</commit_message>
<xml_diff>
--- a/data/my_world.xlsx
+++ b/data/my_world.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>switzerland</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>egypt</t>
+  </si>
+  <si>
+    <t>united states</t>
+  </si>
+  <si>
+    <t>Country1</t>
+  </si>
+  <si>
+    <t>Country2</t>
   </si>
 </sst>
 </file>
@@ -474,115 +483,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B2" t="str">
+        <f>PROPER(A2)</f>
+        <v>Austria</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="B3" t="str">
+        <f>PROPER(A3)</f>
+        <v>Brunei</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="B4" t="str">
+        <f>PROPER(A4)</f>
+        <v>Cambodia</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="B5" t="str">
+        <f>PROPER(A5)</f>
+        <v>Croatia</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="B6" t="str">
+        <f>PROPER(A6)</f>
+        <v>Egypt</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="B7" t="str">
+        <f>PROPER(A7)</f>
+        <v>France</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+      <c r="B8" t="str">
+        <f>PROPER(A8)</f>
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+      <c r="B9" t="str">
+        <f>PROPER(A9)</f>
+        <v>Hong Kong</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
+      <c r="B10" t="str">
+        <f>PROPER(A10)</f>
+        <v>Hungary</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+      <c r="B11" t="str">
+        <f>PROPER(A11)</f>
+        <v>Indonesia</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
+      <c r="B12" t="str">
+        <f>PROPER(A12)</f>
+        <v>Italy</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
+      <c r="B13" t="str">
+        <f>PROPER(A13)</f>
+        <v>Malaysia</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+      <c r="B14" t="str">
+        <f>PROPER(A14)</f>
+        <v>Philippines</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
+      <c r="B15" t="str">
+        <f>PROPER(A15)</f>
+        <v>Qatar</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+      <c r="B16" t="str">
+        <f>PROPER(A16)</f>
+        <v>Singapore</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="B17" t="str">
+        <f>PROPER(A17)</f>
+        <v>Slovenia</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="B18" t="str">
+        <f>PROPER(A18)</f>
+        <v>Spain</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+      <c r="B19" t="str">
+        <f>PROPER(A19)</f>
+        <v>Switzerland</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+      <c r="B20" t="str">
+        <f>PROPER(A20)</f>
+        <v>Thailand</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+      <c r="B21" t="str">
+        <f>PROPER(A21)</f>
+        <v>United Kingdom</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <f>PROPER(A22)</f>
+        <v>United States</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>10</v>
+      </c>
+      <c r="B23" t="str">
+        <f>PROPER(A23)</f>
+        <v>Vietnam</v>
       </c>
     </row>
   </sheetData>

</xml_diff>